<commit_message>
Fix timeout download files
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_10_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_10_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>554/SUP FES 1</v>
+        <v>800/SUP 1</v>
       </c>
       <c r="B2" t="str">
         <v>Supervision</v>
       </c>
       <c r="C2" t="str">
-        <v>D524564</v>
+        <v>J2545456</v>
       </c>
       <c r="D2" t="str">
-        <v>SAMIRA TATA</v>
+        <v>JALAL MED</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -447,16 +447,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H2">
-        <v>10000</v>
+        <v>8000</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1500</v>
+        <v>800</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -467,25 +467,25 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2" t="str">
-        <v>--</v>
+      <c r="N2">
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>8500</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve">044/LF/FES VILLE </v>
+        <v xml:space="preserve">901/FES </v>
       </c>
       <c r="B3" t="str">
-        <v>Logement de fonction</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>L3578354</v>
+        <v>J207703</v>
       </c>
       <c r="D3" t="str">
-        <v>NABIL KAMAL</v>
+        <v>ACHENGLI LAILA</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -494,16 +494,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -518,21 +518,21 @@
         <v>--</v>
       </c>
       <c r="O3">
-        <v>8500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve">044/FES VILLE </v>
+        <v xml:space="preserve">901/LF/FES </v>
       </c>
       <c r="B4" t="str">
-        <v>Direction régionale</v>
+        <v>Logement de fonction</v>
       </c>
       <c r="C4" t="str">
-        <v>K5443645</v>
+        <v>BJ36877</v>
       </c>
       <c r="D4" t="str">
-        <v>KHADIJA LALA</v>
+        <v>CHARIJI ABDELLAH</v>
       </c>
       <c r="E4" t="str">
         <v>non</v>
@@ -541,16 +541,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -565,39 +565,39 @@
         <v>--</v>
       </c>
       <c r="O4">
-        <v>8500</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>800/PV FES 1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B5" t="str">
-        <v>Point de vente</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <v>P5874857</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D5" t="str">
-        <v>KARIM JALAL</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E5" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>15</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G5" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H5">
-        <v>10000</v>
+        <v>19000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1500</v>
+        <v>1900</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -608,63 +608,16 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" t="str">
-        <v>--</v>
+      <c r="N5">
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>8500</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H6">
-        <v>40000</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>6000</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>34000</v>
+        <v>17100</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix maquette telepaiement issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_10_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_10_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>908/DIRECTION REGIONALE SUD</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B2" t="str">
-        <v>Direction régionale</v>
+        <v>Point de vente</v>
       </c>
       <c r="C2" t="str">
-        <v>J207703</v>
+        <v>I83603</v>
       </c>
       <c r="D2" t="str">
-        <v>ACHENGLI LAILA</v>
+        <v>MOHAMED BADRANE</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -447,16 +447,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>20000</v>
+        <v>446.42</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -471,21 +471,21 @@
         <v>--</v>
       </c>
       <c r="O2">
-        <v>17000</v>
+        <v>446.42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>805/KOUTOUBIA</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B3" t="str">
         <v>Point de vente</v>
       </c>
       <c r="C3" t="str">
-        <v>L234567</v>
+        <v>B219321</v>
       </c>
       <c r="D3" t="str">
-        <v>NACER YASSINE</v>
+        <v>JEMAA HORMI</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -494,16 +494,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>12000</v>
+        <v>1250</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -518,21 +518,21 @@
         <v>--</v>
       </c>
       <c r="O3">
-        <v>10200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>900/PATIO</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B4" t="str">
-        <v>Siège</v>
+        <v>Point de vente</v>
       </c>
       <c r="C4" t="str">
-        <v>J207703</v>
+        <v>BK646476</v>
       </c>
       <c r="D4" t="str">
-        <v>ACHENGLI LAILA</v>
+        <v>DOUNIA LAMKADDAM</v>
       </c>
       <c r="E4" t="str">
         <v>non</v>
@@ -541,16 +541,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>4500</v>
+        <v>937.5</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -565,21 +565,21 @@
         <v>--</v>
       </c>
       <c r="O4">
-        <v>4050</v>
+        <v>937.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>908/LF/DIRECTION REGIONALE SUD</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B5" t="str">
-        <v>Logement de fonction</v>
+        <v>Point de vente</v>
       </c>
       <c r="C5" t="str">
-        <v>354646</v>
+        <v>CIN605</v>
       </c>
       <c r="D5" t="str">
-        <v>SOCIETE 1</v>
+        <v>SOFIA BADRANE</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -591,13 +591,13 @@
         <v>10</v>
       </c>
       <c r="H5">
-        <v>8000</v>
+        <v>3750</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>800</v>
+        <v>375</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -612,21 +612,21 @@
         <v>--</v>
       </c>
       <c r="O5">
-        <v>7200</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>908/LF/DIRECTION REGIONALE SUD</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B6" t="str">
-        <v>Logement de fonction</v>
+        <v>Point de vente</v>
       </c>
       <c r="C6" t="str">
-        <v>B12346</v>
+        <v>I150156</v>
       </c>
       <c r="D6" t="str">
-        <v>BAKKALI MOHAMED</v>
+        <v>LATIFA BADRANE</v>
       </c>
       <c r="E6" t="str">
         <v>non</v>
@@ -635,16 +635,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>6000</v>
+        <v>223.21</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -659,21 +659,21 @@
         <v>--</v>
       </c>
       <c r="O6">
-        <v>5400</v>
+        <v>223.21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>908/LF/DIRECTION REGIONALE SUD</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B7" t="str">
-        <v>Logement de fonction</v>
+        <v>Point de vente</v>
       </c>
       <c r="C7" t="str">
-        <v>L234567</v>
+        <v>B171710</v>
       </c>
       <c r="D7" t="str">
-        <v>NACER YASSINE</v>
+        <v>NADIA BADRANE</v>
       </c>
       <c r="E7" t="str">
         <v>non</v>
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>2000</v>
+        <v>223.21</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -706,24 +706,24 @@
         <v>--</v>
       </c>
       <c r="O7">
-        <v>2000</v>
+        <v>223.21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>001/SUP SUD</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B8" t="str">
-        <v>Supervision</v>
+        <v>Point de vente</v>
       </c>
       <c r="C8" t="str">
-        <v>354646</v>
+        <v>Q194939</v>
       </c>
       <c r="D8" t="str">
-        <v>SOCIETE 1</v>
+        <v>OUAFA BADRANE</v>
       </c>
       <c r="E8" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F8" t="str">
         <v>mensuelle</v>
@@ -732,7 +732,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>2400</v>
+        <v>223.21</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -753,21 +753,21 @@
         <v>--</v>
       </c>
       <c r="O8">
-        <v>2400</v>
+        <v>223.21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>389/AOURIR</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B9" t="str">
         <v>Point de vente</v>
       </c>
       <c r="C9" t="str">
-        <v>BJ36877</v>
+        <v>I210578</v>
       </c>
       <c r="D9" t="str">
-        <v>CHARIJI ABDELLAH</v>
+        <v>SAID BADRANE</v>
       </c>
       <c r="E9" t="str">
         <v>non</v>
@@ -776,16 +776,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>7000</v>
+        <v>446.45</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -800,59 +800,247 @@
         <v>--</v>
       </c>
       <c r="O9">
-        <v>6300</v>
+        <v>446.45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
+        <v>052/FKIH BEN SALEH</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C10" t="str">
+        <v>IB19558</v>
+      </c>
+      <c r="D10" t="str">
+        <v>ZERNAKH ABDELLAH</v>
+      </c>
+      <c r="E10" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F10" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>11000</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="str">
+        <v>--</v>
+      </c>
+      <c r="O10">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>052/FKIH BEN SALEH</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C11" t="str">
+        <v>IB43905</v>
+      </c>
+      <c r="D11" t="str">
+        <v>NHILA BELGACEM</v>
+      </c>
+      <c r="E11" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="str">
+        <v>--</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>905/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Q251990</v>
+      </c>
+      <c r="D12" t="str">
+        <v>NOUBAIL MOUNTASSIR</v>
+      </c>
+      <c r="E12" t="str">
+        <v>non</v>
+      </c>
+      <c r="F12" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>6750</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>675</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="str">
+        <v>--</v>
+      </c>
+      <c r="O12">
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>905/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C13" t="str">
+        <v>IR801997</v>
+      </c>
+      <c r="D13" t="str">
+        <v>NOUBAIL MOHAMMED</v>
+      </c>
+      <c r="E13" t="str">
+        <v>non</v>
+      </c>
+      <c r="F13" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>6750</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>675</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="str">
+        <v>--</v>
+      </c>
+      <c r="O13">
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B10" t="str">
+      <c r="B14" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C10" t="str">
+      <c r="C14" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D10" t="str">
+      <c r="D14" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E10" t="str">
+      <c r="E14" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F10" t="str">
+      <c r="F14" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G10" t="str">
+      <c r="G14" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H10">
-        <v>61900</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>7350</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>54550</v>
+      <c r="H14">
+        <v>32000</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>1725</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>30275</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix contrat AV (Deces, Cession, Revision loyer) and multiple proprietaires have same mandataire error
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_10_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_10_2022.xlsx
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>901/CASABLANCA</v>
+        <v>001/TTT/AV1</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>B219321</v>
       </c>
       <c r="D2" t="str">
-        <v>NASIRI HASNAA</v>
+        <v>JEMAA HORMI</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -447,16 +447,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>2666.67</v>
+        <v>2000</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>266.67</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -471,21 +471,21 @@
         <v>--</v>
       </c>
       <c r="O2">
-        <v>2400</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>901/CASABLANCA</v>
+        <v>001/TTT/AV1</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>CIN605</v>
+        <v>IR801997</v>
       </c>
       <c r="D3" t="str">
-        <v>SOFIA BADRANE</v>
+        <v>NOUBAIL MOHAMMED</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -494,16 +494,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>2666.67</v>
+        <v>2000</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>266.67</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -518,21 +518,21 @@
         <v>--</v>
       </c>
       <c r="O3">
-        <v>2400</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>901/CASABLANCA</v>
+        <v>001/TTT/AV1</v>
       </c>
       <c r="B4" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>BK646476</v>
+        <v>IB19558</v>
       </c>
       <c r="D4" t="str">
-        <v>DOUNIA LAMKADDAM</v>
+        <v>ZERNAKH ABDELLAH</v>
       </c>
       <c r="E4" t="str">
         <v>non</v>
@@ -541,16 +541,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>2666.67</v>
+        <v>2000</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>266.67</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -565,7 +565,7 @@
         <v>--</v>
       </c>
       <c r="O4">
-        <v>2400</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5">
@@ -591,13 +591,13 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="H5">
-        <v>8000.01</v>
+        <v>6000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>800.01</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>7200</v>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>